<commit_message>
download hasil ujian pilgan
</commit_message>
<xml_diff>
--- a/public/be_assets/exam/tempImportExam.xlsx
+++ b/public/be_assets/exam/tempImportExam.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="41">
   <si>
     <t>KODE</t>
   </si>
@@ -29,49 +29,115 @@
     <t>JAWABAN</t>
   </si>
   <si>
-    <t>9fc8747327</t>
+    <t>d81566702c</t>
   </si>
   <si>
     <t>Soal</t>
   </si>
   <si>
+    <t>Satu tambah satu hasilnya dua berapa hayo</t>
+  </si>
+  <si>
     <t>option</t>
   </si>
   <si>
-    <t>ea4c51af01</t>
-  </si>
-  <si>
-    <t>s</t>
-  </si>
-  <si>
-    <t>d</t>
-  </si>
-  <si>
-    <t>f</t>
-  </si>
-  <si>
-    <t>g</t>
-  </si>
-  <si>
-    <t>h</t>
-  </si>
-  <si>
-    <t>0a8e95c43c</t>
-  </si>
-  <si>
-    <t>x</t>
-  </si>
-  <si>
-    <t>be_assets\exam\exam_2730d205-308c-4b7f-8f1a-e344b893b7a7.jpeg</t>
-  </si>
-  <si>
-    <t>be_assets\exam\exam_c7b09549-68b6-4005-97d8-16d08884aeb2.jpeg</t>
-  </si>
-  <si>
-    <t>be_assets\exam\exam_6453ba52-77d8-4c48-b94d-42833a2d3f6e.jpeg</t>
-  </si>
-  <si>
-    <t>be_assets\exam\exam_59845ae0-63f3-4fb7-a20f-3d430e11e88d.png</t>
+    <t>satu</t>
+  </si>
+  <si>
+    <t>dua</t>
+  </si>
+  <si>
+    <t>tiga</t>
+  </si>
+  <si>
+    <t>empat</t>
+  </si>
+  <si>
+    <t>lima puluh</t>
+  </si>
+  <si>
+    <t>9a1ffa509a</t>
+  </si>
+  <si>
+    <t>Saya suka makan buah buahan seperti buah naga dan stroberi. Buah apa yang tidak saya sukai ?</t>
+  </si>
+  <si>
+    <t>buah naga</t>
+  </si>
+  <si>
+    <t>buah stroberi</t>
+  </si>
+  <si>
+    <t>buah apel</t>
+  </si>
+  <si>
+    <t>buah durian</t>
+  </si>
+  <si>
+    <t>buah busuk</t>
+  </si>
+  <si>
+    <t>1bba26e08d</t>
+  </si>
+  <si>
+    <t>Bendera indonesia</t>
+  </si>
+  <si>
+    <t>Bendera Jepang</t>
+  </si>
+  <si>
+    <t>Bendera ?</t>
+  </si>
+  <si>
+    <t>Itu Apel</t>
+  </si>
+  <si>
+    <t>Kelereng api</t>
+  </si>
+  <si>
+    <t>13b5a4fd66</t>
+  </si>
+  <si>
+    <t>Kopi kapal apa yang ada apinya ?</t>
+  </si>
+  <si>
+    <t>kopiyama</t>
+  </si>
+  <si>
+    <t>kopiyah</t>
+  </si>
+  <si>
+    <t>kopi kapal api</t>
+  </si>
+  <si>
+    <t>kopiko</t>
+  </si>
+  <si>
+    <t>koko</t>
+  </si>
+  <si>
+    <t>2902a1814d</t>
+  </si>
+  <si>
+    <t>Buat ini mudah</t>
+  </si>
+  <si>
+    <t>ok</t>
+  </si>
+  <si>
+    <t>ya</t>
+  </si>
+  <si>
+    <t>siap</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>ashyaaap</t>
+  </si>
+  <si>
+    <t>be_assets\exam\exam_f176d8ac-4283-4bfc-8f36-e58d89378d6e.png</t>
   </si>
 </sst>
 </file>
@@ -127,15 +193,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1676400</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>1228725</xdr:rowOff>
+      <xdr:colOff>1247775</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -152,118 +218,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm rot="0">
-          <a:ext cx="1638300" cy="1219200"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>66675</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>1409700</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>1143000</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 4" descr=""/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm rot="0">
-          <a:ext cx="1343025" cy="1114425"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>1800225</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>2343150</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 6" descr=""/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm rot="0">
-          <a:ext cx="1790700" cy="2257425"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>828675</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>333375</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 8" descr=""/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm rot="0">
-          <a:ext cx="828675" cy="333375"/>
+          <a:ext cx="1247775" cy="933450"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -565,15 +520,15 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="L9" sqref="L9"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="3" max="3" width="28.85546875" customWidth="true" style="0"/>
+    <col min="3" max="3" width="30.28515625" customWidth="true" style="0"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -590,7 +545,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" customHeight="1" ht="99">
+    <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -598,16 +553,16 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="1"/>
       <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -616,10 +571,10 @@
     <row r="4" spans="1:4">
       <c r="A4" s="1"/>
       <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4">
-        <v>2</v>
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -628,22 +583,22 @@
     <row r="5" spans="1:4">
       <c r="A5" s="1"/>
       <c r="B5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5">
-        <v>3</v>
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
       </c>
       <c r="D5">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:4" customHeight="1" ht="91.5">
+    <row r="6" spans="1:4">
       <c r="A6" s="1"/>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -652,33 +607,33 @@
     <row r="7" spans="1:4">
       <c r="A7" s="1"/>
       <c r="B7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7">
-        <v>5</v>
+        <v>7</v>
+      </c>
+      <c r="C7" t="s">
+        <v>12</v>
       </c>
       <c r="D7">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:4" customHeight="1" ht="28.5">
+    <row r="8" spans="1:4">
       <c r="A8" s="1" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="B8" t="s">
         <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="1"/>
       <c r="B9" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="D9">
         <v>0</v>
@@ -687,22 +642,22 @@
     <row r="10" spans="1:4">
       <c r="A10" s="1"/>
       <c r="B10" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C10" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="D10">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="1"/>
       <c r="B11" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C11" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="D11">
         <v>0</v>
@@ -711,10 +666,10 @@
     <row r="12" spans="1:4">
       <c r="A12" s="1"/>
       <c r="B12" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C12" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="D12">
         <v>0</v>
@@ -723,45 +678,45 @@
     <row r="13" spans="1:4">
       <c r="A13" s="1"/>
       <c r="B13" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C13" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="D13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" customHeight="1" ht="184.5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" customHeight="1" ht="73.5">
       <c r="A14" s="1" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="B14" t="s">
         <v>5</v>
       </c>
       <c r="C14" t="s">
-        <v>17</v>
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="1"/>
       <c r="B15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C15">
-        <v>3</v>
+        <v>7</v>
+      </c>
+      <c r="C15" t="s">
+        <v>21</v>
       </c>
       <c r="D15">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="1"/>
       <c r="B16" t="s">
-        <v>6</v>
-      </c>
-      <c r="C16">
-        <v>4</v>
+        <v>7</v>
+      </c>
+      <c r="C16" t="s">
+        <v>22</v>
       </c>
       <c r="D16">
         <v>0</v>
@@ -770,10 +725,10 @@
     <row r="17" spans="1:4">
       <c r="A17" s="1"/>
       <c r="B17" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C17" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="D17">
         <v>0</v>
@@ -782,10 +737,10 @@
     <row r="18" spans="1:4">
       <c r="A18" s="1"/>
       <c r="B18" t="s">
-        <v>6</v>
-      </c>
-      <c r="C18">
-        <v>6</v>
+        <v>7</v>
+      </c>
+      <c r="C18" t="s">
+        <v>24</v>
       </c>
       <c r="D18">
         <v>0</v>
@@ -794,13 +749,155 @@
     <row r="19" spans="1:4">
       <c r="A19" s="1"/>
       <c r="B19" t="s">
-        <v>6</v>
-      </c>
-      <c r="C19">
-        <v>7</v>
+        <v>7</v>
+      </c>
+      <c r="C19" t="s">
+        <v>25</v>
       </c>
       <c r="D19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="1"/>
+      <c r="B21" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" t="s">
+        <v>28</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="1"/>
+      <c r="B22" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22" t="s">
+        <v>29</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="1"/>
+      <c r="B23" t="s">
+        <v>7</v>
+      </c>
+      <c r="C23" t="s">
+        <v>30</v>
+      </c>
+      <c r="D23">
         <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="1"/>
+      <c r="B24" t="s">
+        <v>7</v>
+      </c>
+      <c r="C24" t="s">
+        <v>31</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" s="1"/>
+      <c r="B25" t="s">
+        <v>7</v>
+      </c>
+      <c r="C25" t="s">
+        <v>32</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B26" t="s">
+        <v>5</v>
+      </c>
+      <c r="C26" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" s="1"/>
+      <c r="B27" t="s">
+        <v>7</v>
+      </c>
+      <c r="C27" t="s">
+        <v>35</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" s="1"/>
+      <c r="B28" t="s">
+        <v>7</v>
+      </c>
+      <c r="C28" t="s">
+        <v>36</v>
+      </c>
+      <c r="D28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" s="1"/>
+      <c r="B29" t="s">
+        <v>7</v>
+      </c>
+      <c r="C29" t="s">
+        <v>37</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" s="1"/>
+      <c r="B30" t="s">
+        <v>7</v>
+      </c>
+      <c r="C30" t="s">
+        <v>38</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" s="1"/>
+      <c r="B31" t="s">
+        <v>7</v>
+      </c>
+      <c r="C31" t="s">
+        <v>39</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -808,6 +905,8 @@
     <mergeCell ref="A2:A7"/>
     <mergeCell ref="A8:A13"/>
     <mergeCell ref="A14:A19"/>
+    <mergeCell ref="A20:A25"/>
+    <mergeCell ref="A26:A31"/>
   </mergeCells>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>